<commit_message>
Updated bug in custom ODE function and included two example notebooks with custom ODEs.
</commit_message>
<xml_diff>
--- a/docs/notebooks/data/fedbatch_fedbatch1_testing_batchdata.xlsx
+++ b/docs/notebooks/data/fedbatch_fedbatch1_testing_batchdata.xlsx
@@ -468,16 +468,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2037148833171987</v>
+        <v>0.267448079705191</v>
       </c>
       <c r="D2" t="n">
-        <v>62.24872802469813</v>
+        <v>56.59964947207498</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1783640750866079</v>
+        <v>0.1278662199799618</v>
       </c>
       <c r="F2" t="n">
-        <v>4.017967202564075</v>
+        <v>0.602540373712727</v>
       </c>
     </row>
     <row r="3">
@@ -488,16 +488,16 @@
         <v>4.210526315789473</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2435010902287608</v>
+        <v>0.3149671924479802</v>
       </c>
       <c r="D3" t="n">
-        <v>59.15949792686844</v>
+        <v>41.96729235941639</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5675025526327994</v>
+        <v>2.450578998413719</v>
       </c>
       <c r="F3" t="n">
-        <v>4.228493518353549</v>
+        <v>0.8130666895022006</v>
       </c>
     </row>
     <row r="4">
@@ -508,16 +508,16 @@
         <v>8.421052631578947</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3284695469044285</v>
+        <v>0.4717942581390715</v>
       </c>
       <c r="D4" t="n">
-        <v>56.37309103471762</v>
+        <v>33.38091580073113</v>
       </c>
       <c r="E4" t="n">
-        <v>0.821816497379465</v>
+        <v>3.559937583522633</v>
       </c>
       <c r="F4" t="n">
-        <v>4.439019834143022</v>
+        <v>1.023593005291674</v>
       </c>
     </row>
     <row r="5">
@@ -528,16 +528,16 @@
         <v>12.63157894736842</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4661307119061669</v>
+        <v>0.7564205904828479</v>
       </c>
       <c r="D5" t="n">
-        <v>53.85108408086009</v>
+        <v>27.75244887172457</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9323270712251929</v>
+        <v>3.929490631381696</v>
       </c>
       <c r="F5" t="n">
-        <v>4.649546149932496</v>
+        <v>1.234119321081148</v>
       </c>
     </row>
     <row r="6">
@@ -548,16 +548,16 @@
         <v>16.84210526315789</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6677019016349858</v>
+        <v>1.269833776201699</v>
       </c>
       <c r="D6" t="n">
-        <v>51.56274117981751</v>
+        <v>23.83950404212584</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8815905502993293</v>
+        <v>3.565748507366222</v>
       </c>
       <c r="F6" t="n">
-        <v>4.860072465721969</v>
+        <v>1.444645636870622</v>
       </c>
     </row>
     <row r="7">
@@ -568,16 +568,16 @@
         <v>21.05263157894737</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9281864050651976</v>
+        <v>2.088060297240443</v>
       </c>
       <c r="D7" t="n">
-        <v>49.47954851620818</v>
+        <v>21.00339382255697</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6837642420872594</v>
+        <v>2.424632906425339</v>
       </c>
       <c r="F7" t="n">
-        <v>5.070598781511443</v>
+        <v>1.655171952660095</v>
       </c>
     </row>
     <row r="8">
@@ -588,16 +588,16 @@
         <v>25.26315789473684</v>
       </c>
       <c r="C8" t="n">
-        <v>1.202536059833841</v>
+        <v>3.077717856651489</v>
       </c>
       <c r="D8" t="n">
-        <v>47.56936927436864</v>
+        <v>18.87752502011085</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4324444089877149</v>
+        <v>0.8290374915218717</v>
       </c>
       <c r="F8" t="n">
-        <v>5.281125097300917</v>
+        <v>1.865698268449569</v>
       </c>
     </row>
     <row r="9">
@@ -608,16 +608,16 @@
         <v>29.47368421052632</v>
       </c>
       <c r="C9" t="n">
-        <v>1.427754454545161</v>
+        <v>3.529408070698828</v>
       </c>
       <c r="D9" t="n">
-        <v>45.80002822765291</v>
+        <v>17.11612189554089</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2565863869787361</v>
+        <v>0.2314275584648205</v>
       </c>
       <c r="F9" t="n">
-        <v>5.49165141309039</v>
+        <v>2.076224584239043</v>
       </c>
     </row>
     <row r="10">
@@ -628,16 +628,16 @@
         <v>33.68421052631579</v>
       </c>
       <c r="C10" t="n">
-        <v>1.593240725795179</v>
+        <v>3.681295558283151</v>
       </c>
       <c r="D10" t="n">
-        <v>44.15271568055753</v>
+        <v>15.63571503292816</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1799176012720223</v>
+        <v>0.1771222661167388</v>
       </c>
       <c r="F10" t="n">
-        <v>5.702177728879865</v>
+        <v>2.286750900028516</v>
       </c>
     </row>
     <row r="11">
@@ -648,16 +648,16 @@
         <v>37.89473684210526</v>
       </c>
       <c r="C11" t="n">
-        <v>1.727499544555397</v>
+        <v>3.796827757929666</v>
       </c>
       <c r="D11" t="n">
-        <v>42.61882219470806</v>
+        <v>14.40276247053303</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1475943611260985</v>
+        <v>0.15346578630132</v>
       </c>
       <c r="F11" t="n">
-        <v>5.912704044669339</v>
+        <v>2.497277215817989</v>
       </c>
     </row>
     <row r="12">
@@ -668,16 +668,16 @@
         <v>42.10526315789473</v>
       </c>
       <c r="C12" t="n">
-        <v>1.846875227883147</v>
+        <v>3.893371298411551</v>
       </c>
       <c r="D12" t="n">
-        <v>41.18927383881763</v>
+        <v>13.36132434918641</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1287959214725349</v>
+        <v>0.1355355192930273</v>
       </c>
       <c r="F12" t="n">
-        <v>6.123230360458812</v>
+        <v>2.707803531607463</v>
       </c>
     </row>
     <row r="13">
@@ -688,16 +688,16 @@
         <v>46.31578947368421</v>
       </c>
       <c r="C13" t="n">
-        <v>1.956323344284391</v>
+        <v>3.975382378184309</v>
       </c>
       <c r="D13" t="n">
-        <v>39.85436000839648</v>
+        <v>12.47002278048386</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1152306830680628</v>
+        <v>0.1213987975567884</v>
       </c>
       <c r="F13" t="n">
-        <v>6.333756676248285</v>
+        <v>2.918329847396937</v>
       </c>
     </row>
     <row r="14">
@@ -708,16 +708,16 @@
         <v>50.52631578947368</v>
       </c>
       <c r="C14" t="n">
-        <v>2.057737286990446</v>
+        <v>4.04589578091252</v>
       </c>
       <c r="D14" t="n">
-        <v>38.60513472872117</v>
+        <v>11.6985721139952</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1045229999830395</v>
+        <v>0.1100872244624954</v>
       </c>
       <c r="F14" t="n">
-        <v>6.544282992037759</v>
+        <v>3.128856163186411</v>
       </c>
     </row>
     <row r="15">
@@ -728,16 +728,16 @@
         <v>54.73684210526316</v>
       </c>
       <c r="C15" t="n">
-        <v>2.152198756660972</v>
+        <v>4.107201075838239</v>
       </c>
       <c r="D15" t="n">
-        <v>37.43365216134531</v>
+        <v>11.02432787683328</v>
       </c>
       <c r="E15" t="n">
-        <v>0.09574468904220901</v>
+        <v>0.1008364647788515</v>
       </c>
       <c r="F15" t="n">
-        <v>6.754809307827233</v>
+        <v>3.339382478975885</v>
       </c>
     </row>
     <row r="16">
@@ -748,16 +748,16 @@
         <v>58.94736842105263</v>
       </c>
       <c r="C16" t="n">
-        <v>2.240522646756836</v>
+        <v>4.161153794865354</v>
       </c>
       <c r="D16" t="n">
-        <v>36.33289991112127</v>
+        <v>10.43003911632785</v>
       </c>
       <c r="E16" t="n">
-        <v>0.08835184399556577</v>
+        <v>0.09284531370782054</v>
       </c>
       <c r="F16" t="n">
-        <v>6.965335623616706</v>
+        <v>3.549908794765359</v>
       </c>
     </row>
     <row r="17">
@@ -768,16 +768,16 @@
         <v>63.1578947368421</v>
       </c>
       <c r="C17" t="n">
-        <v>2.32334686314293</v>
+        <v>4.208935264265145</v>
       </c>
       <c r="D17" t="n">
-        <v>35.29667223726661</v>
+        <v>9.902266304978705</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0820271023945329</v>
+        <v>0.08600934679737154</v>
       </c>
       <c r="F17" t="n">
-        <v>7.17586193940618</v>
+        <v>3.760435110554833</v>
       </c>
     </row>
     <row r="18">
@@ -788,16 +788,16 @@
         <v>67.36842105263158</v>
       </c>
       <c r="C18" t="n">
-        <v>2.401191819506123</v>
+        <v>4.251539985907844</v>
       </c>
       <c r="D18" t="n">
-        <v>34.31946194820772</v>
+        <v>9.430432716551824</v>
       </c>
       <c r="E18" t="n">
-        <v>0.07657881552199949</v>
+        <v>0.08011889574567313</v>
       </c>
       <c r="F18" t="n">
-        <v>7.386388255195653</v>
+        <v>3.970961426344306</v>
       </c>
     </row>
     <row r="19">
@@ -808,16 +808,16 @@
         <v>71.57894736842105</v>
       </c>
       <c r="C19" t="n">
-        <v>2.474504210661007</v>
+        <v>4.289756738139515</v>
       </c>
       <c r="D19" t="n">
-        <v>33.39636910694175</v>
+        <v>9.006090572991207</v>
       </c>
       <c r="E19" t="n">
-        <v>0.07186864267836592</v>
+        <v>0.0750174006789331</v>
       </c>
       <c r="F19" t="n">
-        <v>7.596914570985128</v>
+        <v>4.18148774213378</v>
       </c>
     </row>
     <row r="20">
@@ -828,16 +828,16 @@
         <v>75.78947368421052</v>
       </c>
       <c r="C20" t="n">
-        <v>2.543680905080736</v>
+        <v>4.324250590989138</v>
       </c>
       <c r="D20" t="n">
-        <v>32.52302194988601</v>
+        <v>8.622417339452518</v>
       </c>
       <c r="E20" t="n">
-        <v>0.06777645696811314</v>
+        <v>0.07052326305925839</v>
       </c>
       <c r="F20" t="n">
-        <v>7.807440886774601</v>
+        <v>4.392014057923253</v>
       </c>
     </row>
     <row r="21">
@@ -848,16 +848,16 @@
         <v>80</v>
       </c>
       <c r="C21" t="n">
-        <v>2.609126124480566</v>
+        <v>4.355492648673713</v>
       </c>
       <c r="D21" t="n">
-        <v>31.69551767660233</v>
+        <v>8.273824312724505</v>
       </c>
       <c r="E21" t="n">
-        <v>0.06409667732964447</v>
+        <v>0.06663267261113104</v>
       </c>
       <c r="F21" t="n">
-        <v>8.017967202564074</v>
+        <v>4.602540373712726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>